<commit_message>
Added materials for unstack using pivotby
</commit_message>
<xml_diff>
--- a/Excel/YouTube Materials/Rolling aggregates/Owen Price - Excel - Demonstration of rolling aggregates.xlsx
+++ b/Excel/YouTube Materials/Rolling aggregates/Owen Price - Excel - Demonstration of rolling aggregates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62a07d598bdbd2d4/Documents/Blog/Content/Excel/rolling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62a07d598bdbd2d4/Documents/Blog/Projects/Social content/Excel/YouTube Materials/Rolling aggregates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="535" documentId="13_ncr:1_{FFDBAB9C-9074-42D5-B689-1CA42D949907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B92CCC05-88E3-4ABA-944D-5A115F511FFF}"/>
+  <xr:revisionPtr revIDLastSave="545" documentId="13_ncr:1_{FFDBAB9C-9074-42D5-B689-1CA42D949907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EE28C90-D92B-4E82-AD7B-6E30071A113F}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="270" windowWidth="25440" windowHeight="15990" xr2:uid="{DCA575A9-AF13-4812-ABF9-9F6A4A01F50D}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -237,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1356,7 +1356,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="856" row="17">
+  <wetp:taskpane dockstate="right" visibility="0" width="856" row="16">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1392,7 +1392,7 @@
   <dimension ref="B1:P38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>